<commit_message>
ASM Flow Update 26-Aug-25
</commit_message>
<xml_diff>
--- a/password.xlsx
+++ b/password.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E126"/>
+  <dimension ref="A1:E125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,21 +461,21 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Aakash Trading Co|ACUSDA0830</t>
+          <t>Anjani Putra Marketing|ACUSDA0699</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Ankit Bhardwaj</t>
+          <t>Vacant</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>2025</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="3">
@@ -484,21 +484,21 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Abhinandan Enterprises|ACUSDA0088</t>
+          <t>Shree Ji Enterprises|ACUSDS0174</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Brajesh Sharma</t>
+          <t>Hitesh Thakker</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>2025</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="4">
@@ -507,21 +507,21 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Adhira Agency|ACUSDSS005</t>
+          <t>Ishan Marketing|ACUSDI9604</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Shashi Mishra</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1164</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="5">
@@ -530,21 +530,21 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Prabhat Agency|ACUSDP2385</t>
+          <t>Ashok Traders|ACUSDA0117</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Shashi Mishra</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1164</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="6">
@@ -553,21 +553,21 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Aggarwal Agency|ACUSDA0410</t>
+          <t>Khemani Enetrprises (Conf)|ACUSDK2024</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Ankit Bhardwaj</t>
+          <t>Vacant</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>2025</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="7">
@@ -576,21 +576,21 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Ajinkya Traders|ACUSDA0146</t>
+          <t>Proline Sales Agency|ACUSDP5556</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Shailesh Surve</t>
+          <t>Vacant</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>7136</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="8">
@@ -599,21 +599,21 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Amar Nath Harishchand|ACUSDA0133</t>
+          <t>Farr Ayo Distribution|ACUSDF0061</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Parmod Kumar</t>
+          <t>Girvat Raj</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>2025</v>
+        <v>4370</v>
       </c>
     </row>
     <row r="9">
@@ -622,21 +622,21 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Amit Sales|ACUSDA0137</t>
+          <t>Parshvanath Sales Agency|ACUSDP0211</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Anand Gupta</t>
+          <t>Hitesh Thakker</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>2025</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="10">
@@ -645,21 +645,21 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Anand Sales|ACUSDA0820</t>
+          <t>Joshi Enterprises|ACUSDJ0572</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Neeraj Kapoor</t>
+          <t>Vacant</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2025</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="11">
@@ -668,21 +668,21 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Anant Wardrobe|ACUSD00073</t>
+          <t>Raj Sales|ACUSDR4923</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Brajesh Sharma</t>
+          <t>Hitesh Thakker</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>2025</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="12">
@@ -696,16 +696,16 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Farr Ayo Distribution|ACUSDF0061</t>
+          <t>C.J.Malaviya &amp; Co.|ACUSDC0049</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Girvat Raj</t>
+          <t>Hittesh Thakkar</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>4370</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="13">
@@ -719,16 +719,16 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Anjani Putra Marketing|ACUSDA0699</t>
+          <t>Somnath Ji Traders|ACUSDS4925</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Sahil Mansuri</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>1164</v>
+        <v>4760</v>
       </c>
     </row>
     <row r="14">
@@ -737,17 +737,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Uttarakhand</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Ankit Kumar &amp; Brothers|ACUSDA0797</t>
+          <t>Satnam Sales|AQUSDK2024</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Avneesh</t>
+          <t>Yogesh</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -765,12 +765,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Ashish &amp; Co.|ACUSDA1159</t>
+          <t>Madhu Enterprises|ACUSDM0117</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Rakesh Kumar</t>
+          <t>Ajit Pal</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -788,12 +788,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Ashish &amp; Co.|ACUSDA1159</t>
+          <t>Hoseiry House|ACUSDH4804</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Badal Srivastava</t>
+          <t>Ajit Pal</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -806,21 +806,21 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Ashok Traders|ACUSDA0117</t>
+          <t>Shree Kanha Ji Marketing|ACUSDS0438</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Toshif Mansuri</t>
+          <t>Rajiv Kumar</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>9989</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="18">
@@ -829,21 +829,21 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Ishan Marketing|ACUSDI9604</t>
+          <t>Shreyansh Marketing|ACUSDS0070</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Toshif Mansuri</t>
+          <t>Mahesh</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>9989</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="19">
@@ -852,17 +852,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Bajarang Sweet House (Conf)|ACUSDB0963</t>
+          <t>Vishal Traders|ACUSDV0085</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Jasbir Verma</t>
+          <t>Jasbeer Verma</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -875,17 +875,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Barsaiya Traders|ACUSDB0005</t>
+          <t>Ashish &amp; Co.|ACUSDA1159</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Vinay Pandey</t>
+          <t>Badal Srivastava</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -898,17 +898,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Bhagwan Das Kirana And General Store|</t>
+          <t>P.R.Sales Agency|ACUSDP0142</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Vinay Pandey</t>
+          <t>Rakesh Kumar</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -921,15 +921,19 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Bhagwan Das Kirana And General Store|</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr"/>
+          <t>Swastik Enterprises|ACUSDS1206</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Jasbeer Verma</t>
+        </is>
+      </c>
       <c r="E22" t="n">
         <v>2025</v>
       </c>
@@ -940,17 +944,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Bhana Ram &amp; Sons|ACUSDB0473</t>
+          <t>Dalal Trading Co.|ACUSDD1126</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Neeraj Kapoor</t>
+          <t>Yogesh</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -963,21 +967,21 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Bharat Traders|ACUSDB0039</t>
+          <t>Shri Radhey Krishna Trading Co.|ACUSDS1204</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Kapil Sharma</t>
+          <t>Jasbeer Verma</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>4920</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="25">
@@ -986,21 +990,21 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Shree Datta Agency|ACUSDSS004</t>
+          <t>Vishal Trading Co.|ACUSDV0079</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Pradeep Kumar</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>1164</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="26">
@@ -1009,21 +1013,21 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>C.J.Malaviya &amp; Co.|ACUSDC0049</t>
+          <t>Shubham Overseas|ACUSDS1407</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Vinesh Trivedi</t>
+          <t>Yogesh</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>3343</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="27">
@@ -1032,17 +1036,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Churaman Biharilal Asati|ACUSDC0531</t>
+          <t>Rameshwarm Enterprises|ACUSDR4921</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Anand Gupta</t>
+          <t>Ajit Pal</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -1055,17 +1059,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Commander Trade Link|ACUSDC1514</t>
+          <t>Pulkit Trading Co.|ACUSDP0132</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Jasbir Verma</t>
+          <t>Badal Srivastava</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -1083,12 +1087,12 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Dalal Trading Co.|ACUSDD1126</t>
+          <t>Paras Kumar Satish Kr|ACUSDP0929</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Raj Kumar</t>
+          <t>Rakesh Kumar</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1101,17 +1105,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Uttarakhand</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Deepak Agency|ACUSDD0543</t>
+          <t>Murli Wala Sales|ACUSDM0200</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Prakash Lohani</t>
+          <t>Mahesh</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -1124,17 +1128,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Deepak Enterprises|ACUSDD0616</t>
+          <t>Kalyani Trading Co.|ACUSDK0087</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Parmod Kumar</t>
+          <t>Ajit Pal</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -1147,17 +1151,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Uttarakhand</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Durga Enterprises (Rishikesh)|ACUSDS0457</t>
+          <t>Harshit Trading Com|ACUSDY0005</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Avneesh</t>
+          <t>Badal Srivastava</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -1170,17 +1174,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Garg Sales Corporation|ACUSDG1091</t>
+          <t>Ravindra Associates|ACUSDR0520</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Neeraj Kapoor</t>
+          <t>Yogesh</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1193,17 +1197,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Goyal Marketing|ACUSDG0603</t>
+          <t>Shakshi Enterprises|ACUSDS0338</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Ankit Bhardwaj</t>
+          <t>Jasbeer Verma</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -1216,17 +1220,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Grace Drinks Pvt Ltd|ACUSDG0174</t>
+          <t>Jai Shri Shyam Traders|LCLSOJ0054</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Shymu Verma</t>
+          <t>Yogesh</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1239,17 +1243,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Uttarakhand</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Hari Enterprises|ACUSDH0073</t>
+          <t>Maruti Enterprises|ACUSDM0088</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Salabh Partap</t>
+          <t>Yogesh</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -1262,17 +1266,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Harshit Trading Com|ACUSDY0005</t>
+          <t>Deepak Enterprises|ACUSDD0616</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Rakesh Kumar</t>
+          <t>Parmod Kumar</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -1285,17 +1289,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Hoseiry House|ACUSDH4804</t>
+          <t>Katna Sales|ACUSDK0086</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Ajit Pal</t>
+          <t>Parmod Kumar</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -1308,21 +1312,21 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>J.K. Brothers|ACUSDJ4838</t>
+          <t>Rattanchand And Sons|ACUSDR0130</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Parmod Kumar</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>1164</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="40">
@@ -1331,21 +1335,21 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Jai Mata Di Agency|ACUSDSS001</t>
+          <t>Amar Nath Harishchand|ACUSDA0133</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Parmod Kumar</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>1164</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="41">
@@ -1354,17 +1358,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Jai Shri Shyam Traders|LCLSOJ0054</t>
+          <t>Shashank Enteprises|ACUSDS4809</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Raj Kumar</t>
+          <t>Parmod Kumar</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1377,21 +1381,21 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Jainil Traders|ACUSDJ0023</t>
+          <t>Vinay Traders|ACUSDV0207</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Sushil Kumar</t>
+          <t>Vinay Pandey</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>2393</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="43">
@@ -1400,17 +1404,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Jeet Ram And Sons|ACUSD00063</t>
+          <t>Anant Wardrobe|ACUSD00073</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Neeraj Kapoor</t>
+          <t>Brajesh Sharma</t>
         </is>
       </c>
       <c r="E43" t="n">
@@ -1423,17 +1427,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Joshi Enterprises|ACUSDJ0572</t>
+          <t>Shree Gopalji Enterprises|ACUSDS2806</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Shashi Mishra</t>
+          <t>Ankit Bhardwaj</t>
         </is>
       </c>
       <c r="E44" t="n">
@@ -1446,17 +1450,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Kalyani Trading Co.|ACUSDK0087</t>
+          <t>Barsaiya Traders|ACUSDB0005</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Ajit Pal</t>
+          <t>Vinay Pandey</t>
         </is>
       </c>
       <c r="E45" t="n">
@@ -1469,17 +1473,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Katna Sales|ACUSDK0086</t>
+          <t>Goyal Marketing|ACUSDG0603</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Parmod Kumar</t>
+          <t>Ankit Bhardwaj</t>
         </is>
       </c>
       <c r="E46" t="n">
@@ -1492,17 +1496,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Khemani Enetrprises (Conf)|ACUSDK2024</t>
+          <t>Parvati Agency|ACUSDP4826</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Shashi Mishra</t>
+          <t>Ankit Bhardwaj</t>
         </is>
       </c>
       <c r="E47" t="n">
@@ -1515,21 +1519,21 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Krishna Agencies|ACUSDSS003</t>
+          <t>Naman Enterprises|ACUSDN1114</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Anand Gupta</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>1164</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="49">
@@ -1543,7 +1547,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Krishna Enterprises|</t>
+          <t>Aakash Trading Co|ACUSDA0830</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1561,17 +1565,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Madhu Enterprises|ACUSDM0117</t>
+          <t>Churaman Biharilal Asati|ACUSDC0531</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Ajit Pal</t>
+          <t>Anand Gupta</t>
         </is>
       </c>
       <c r="E50" t="n">
@@ -1584,17 +1588,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Maruti Enterprises|ACUSDM0088</t>
+          <t>Varun Enterprises|ACUSDV0208</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Parvesh Sharma</t>
+          <t>Vinay Pandey</t>
         </is>
       </c>
       <c r="E51" t="n">
@@ -1607,17 +1611,17 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Uttarakhand</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Mishra Traders- Chamoli(Dewal)|ACUSDM0228</t>
+          <t>Amit Sales|ACUSDA0137</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Premdeep Deshwal</t>
+          <t>Anand Gupta</t>
         </is>
       </c>
       <c r="E52" t="n">
@@ -1630,17 +1634,17 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Murli Wala Sales|ACUSDM0200</t>
+          <t>Shanti Marketing|ACUSDS4808</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Mahesh</t>
+          <t>Vinay Pandey</t>
         </is>
       </c>
       <c r="E53" t="n">
@@ -1653,17 +1657,17 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Uttarakhand</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Naman Agency|ACUSDN0028</t>
+          <t>Abhinandan Enterprises|ACUSDA0088</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Avneesh</t>
+          <t>Brajesh Sharma</t>
         </is>
       </c>
       <c r="E54" t="n">
@@ -1681,12 +1685,12 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Naman Enterprises|ACUSDN1114</t>
+          <t>O.S. Agency|ACUSDO0028</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Anand Gupta</t>
+          <t>Vinay Pandey</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -1699,21 +1703,21 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Navinya Enterprises|ACUSDN0052</t>
+          <t>R.D. Plastic|ACUSDR0127</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Shailesh Surve</t>
+          <t>Vinay Pandey</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>7136</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="57">
@@ -1722,21 +1726,21 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Nidhi Sales|ACUSDN4807</t>
+          <t>Krishna Enterprises|</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Anil Jamadar Singh</t>
+          <t>Ankit Bhardwaj</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>5808</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="58">
@@ -1750,12 +1754,12 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>O.S. Agency|ACUSDO0028</t>
+          <t>Aggarwal Agency|ACUSDA0410</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Vinay Pandey</t>
+          <t>Ankit Bhardwaj</t>
         </is>
       </c>
       <c r="E58" t="n">
@@ -1768,21 +1772,21 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Optimize Crusder|ACUSDO0026</t>
+          <t>Bhagwan Das Kirana And General Store|</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Kapil Sharma</t>
+          <t>Vinay Pandey</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>4920</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="60">
@@ -1791,21 +1795,17 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Nidhi Sales|NIDHI SALES</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Anil Jamadar Singh</t>
-        </is>
-      </c>
+          <t>Bhagwan Das Kirana And General Store|</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr"/>
       <c r="E60" t="n">
-        <v>5808</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="61">
@@ -1814,17 +1814,17 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>P.R.Sales Agency|ACUSDP0142</t>
+          <t>Reliable Industry|ACUSDR0204</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Rakesh Kumar</t>
+          <t>Vinay Pandey</t>
         </is>
       </c>
       <c r="E61" t="n">
@@ -1837,17 +1837,17 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Paras Kumar Satish Kr|ACUSDP0929</t>
+          <t>Prabhat Agency|ACUSDP2385</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Rakesh Kumar</t>
+          <t>Rakesh Tripathi</t>
         </is>
       </c>
       <c r="E62" t="n">
@@ -1860,21 +1860,21 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Raj Sales|ACUSDR4923</t>
+          <t>Prabhat Trading Com.|ACUSDP0183</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Hitesh Thakker</t>
+          <t>Anil Jamadar Singh</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>1827</v>
+        <v>5808</v>
       </c>
     </row>
     <row r="64">
@@ -1883,21 +1883,21 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Shree Ji Enterprises|ACUSDS0174</t>
+          <t>Adhira Agency|ACUSDSS005</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Hitesh Thakker</t>
+          <t>Vacant</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>1827</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="65">
@@ -1906,21 +1906,21 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Parshvanath Sales Agency|ACUSDP0211</t>
+          <t>Optimize Crusder|ACUSDO0026</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Hitesh Thakker</t>
+          <t>Kapil Sharma</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>1827</v>
+        <v>4920</v>
       </c>
     </row>
     <row r="66">
@@ -1929,21 +1929,21 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Parvati Agency|ACUSDP4826</t>
+          <t>Jainil Traders|ACUSDJ0023</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Ankit Bhardwaj</t>
+          <t>Vacant</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>2025</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="67">
@@ -1957,16 +1957,16 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Prabhat Trading Com.|ACUSDP0183</t>
+          <t>Krishna Agencies|ACUSDSS003</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Anil Jamadar Singh</t>
+          <t>Vacant</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>5808</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="68">
@@ -1975,21 +1975,21 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Uttarakhand</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Pradeep Agency|ACUSDP4808</t>
+          <t>Bharat Traders|ACUSDB0039</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Prakash Lohani</t>
+          <t>Kapil Sharma</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>2025</v>
+        <v>4920</v>
       </c>
     </row>
     <row r="69">
@@ -1998,21 +1998,21 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Proline Sales Agency|ACUSDP5556</t>
+          <t>J.K. Brothers|ACUSDJ4838</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Shashi Mishra</t>
+          <t>Vacant</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>2025</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="70">
@@ -2021,21 +2021,21 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Pulkit Trading Co.|ACUSDP0132</t>
+          <t>Jai Mata Di Agency|ACUSDSS001</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Rakesh Kumar</t>
+          <t>Vacant</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>2025</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="71">
@@ -2044,21 +2044,21 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>R.D. Plastic|ACUSDR0127</t>
+          <t>Sunrise Enterprises|ACUSDS0771</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Vinay Pandey</t>
+          <t>Dinesh Sharma</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>2025</v>
+        <v>7757</v>
       </c>
     </row>
     <row r="72">
@@ -2067,21 +2067,21 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Rameshwarm Enterprises|ACUSDR4921</t>
+          <t>Nidhi Sales|ACUSDN4807</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Ajit Pal</t>
+          <t>Anil Jamadar Singh</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>2025</v>
+        <v>5808</v>
       </c>
     </row>
     <row r="73">
@@ -2090,21 +2090,21 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Rattanchand And Sons|ACUSDR0130</t>
+          <t>Krishna Marketing|ACUSDSS006</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Parmod Kumar</t>
+          <t>Vacant</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>2025</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="74">
@@ -2113,21 +2113,21 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Uttarakhand</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Ravi Sons Enterprises|ACUSDR0205</t>
+          <t>Ajinkya Traders|ACUSDA0146</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Prakash Lohani</t>
+          <t>Shailesh Surve</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>2025</v>
+        <v>7136</v>
       </c>
     </row>
     <row r="75">
@@ -2136,17 +2136,17 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Ravindra Associates|ACUSDR0520</t>
+          <t>Tirupati Agencies|ACUSDSS002</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Raj Kumar</t>
+          <t>Rakesh Tripathi</t>
         </is>
       </c>
       <c r="E75" t="n">
@@ -2159,17 +2159,17 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Reliable Industry|ACUSDR0204</t>
+          <t>Shree Datta Agency|ACUSDSS004</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Vinay Pandey</t>
+          <t>Rakesh Tripathi</t>
         </is>
       </c>
       <c r="E76" t="n">
@@ -2182,21 +2182,21 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Sant Enterprises|ACUSDS1100</t>
+          <t>Navinya Enterprises|ACUSDN0052</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Jasbir Verma</t>
+          <t>Shailesh Surve</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>2025</v>
+        <v>7136</v>
       </c>
     </row>
     <row r="78">
@@ -2205,17 +2205,17 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Satnam Sales|AQUSDK2024</t>
+          <t>Garg Sales Corporation|ACUSDG1091</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Parvesh Sharma</t>
+          <t>Neeraj Kapoor</t>
         </is>
       </c>
       <c r="E78" t="n">
@@ -2233,12 +2233,12 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Saurabh Traders|ACUSDSS106</t>
+          <t>Bajarang Sweet House (Conf)|ACUSDB0963</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Rajinder Singh</t>
+          <t>Jasbir Verma</t>
         </is>
       </c>
       <c r="E79" t="n">
@@ -2251,17 +2251,17 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Shakshi Enterprises|ACUSDS0338</t>
+          <t>Sant Enterprises|ACUSDS1100</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Jasbeer Verma</t>
+          <t>Jasbir Verma</t>
         </is>
       </c>
       <c r="E80" t="n">
@@ -2274,17 +2274,17 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Shanti Marketing|ACUSDS4808</t>
+          <t>Shivam Agency|ACUSDSS896</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Vinay Pandey</t>
+          <t>Rajinder Singh</t>
         </is>
       </c>
       <c r="E81" t="n">
@@ -2297,17 +2297,17 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Shashank Enteprises|ACUSDS4809</t>
+          <t>Jeet Ram And Sons|ACUSD00063</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Parmod Kumar</t>
+          <t>Neeraj Kapoor</t>
         </is>
       </c>
       <c r="E82" t="n">
@@ -2325,12 +2325,12 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Shivam Agency|ACUSDSS896</t>
+          <t>Commander Trade Link|ACUSDC1514</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Rajinder Singh</t>
+          <t>Jasbir Verma</t>
         </is>
       </c>
       <c r="E83" t="n">
@@ -2343,17 +2343,17 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Uttarakhand</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Shree Balaji Sales|ACUSDS0202</t>
+          <t>Saurabh Traders|ACUSDSS106</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Salabh Partap</t>
+          <t>Rajinder Singh</t>
         </is>
       </c>
       <c r="E84" t="n">
@@ -2366,17 +2366,17 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Uttarakhand</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Shree Ganesh Agency|ACUSDS1001</t>
+          <t>Suri Enterprises|ACUSD00062</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Salabh Partap</t>
+          <t>Neeraj Kapoor</t>
         </is>
       </c>
       <c r="E85" t="n">
@@ -2389,17 +2389,17 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Shree Gopalji Enterprises|ACUSDS2806</t>
+          <t>Grace Drinks Pvt Ltd|ACUSDG0174</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Ankit Bhardwaj</t>
+          <t>Shymu Verma</t>
         </is>
       </c>
       <c r="E86" t="n">
@@ -2412,17 +2412,17 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Shree Kanha Ji Marketing|ACUSDS0438</t>
+          <t>Suri Enterprises|ACUSD00062</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Rajiv Kumar</t>
+          <t>Shymu Verma</t>
         </is>
       </c>
       <c r="E87" t="n">
@@ -2435,21 +2435,21 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Shree Krishna Marketing|ACUSDSS006</t>
+          <t>Anand Sales|ACUSDA0820</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Neeraj Kapoor</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>1164</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="89">
@@ -2458,17 +2458,17 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Shreyansh Marketing|ACUSDS0070</t>
+          <t>Bhana Ram &amp; Sons|ACUSDB0473</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Mahesh</t>
+          <t>Neeraj Kapoor</t>
         </is>
       </c>
       <c r="E89" t="n">
@@ -2481,21 +2481,21 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Rajasthan</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Shri Radhey Krishna Trading Co.|ACUSDS1204</t>
+          <t>Rasik Remedies Pvt. Ltd.|ACUSDR0074</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Jasbeer Verma</t>
+          <t>Yogesh Sharma</t>
         </is>
       </c>
       <c r="E90" t="n">
-        <v>2025</v>
+        <v>9843</v>
       </c>
     </row>
     <row r="91">
@@ -2504,21 +2504,21 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Rajasthan</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Shubham Overseas|ACUSDS1407</t>
+          <t>Palak Agency|ACUSDP0178</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Satish Singh</t>
         </is>
       </c>
       <c r="E91" t="n">
-        <v>1164</v>
+        <v>6530</v>
       </c>
     </row>
     <row r="92">
@@ -2527,21 +2527,21 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Uttarakhand</t>
+          <t>Rajasthan</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Shyam Sunder Enterprises- Pithoragarh|ACUSDS0462</t>
+          <t>New Sunrise Agency|ACUSDN0605</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Puneet Kansara</t>
         </is>
       </c>
       <c r="E92" t="n">
-        <v>1164</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="93">
@@ -2550,17 +2550,17 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Uttarakhand</t>
+          <t>Rajasthan</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Shyam Sunder Enterprises- Pithoragarh|ACUSDS0462</t>
+          <t>Jai Shankar Agency|ACUSDJ0595</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Prakash Lohani</t>
+          <t>Sarwan Sharma</t>
         </is>
       </c>
       <c r="E93" t="n">
@@ -2573,21 +2573,21 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Rajasthan</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Somnath Ji Traders|ACUSDS4925</t>
+          <t>Shri Vidhan Agency|ACUSDS0364</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Sahil Mansuri</t>
+          <t>Ajay Sachdeva / Ashu Tosh</t>
         </is>
       </c>
       <c r="E94" t="n">
-        <v>4760</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="95">
@@ -2596,21 +2596,21 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Rajasthan</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Sunrise Enterprises|ACUSDS0771</t>
+          <t>Geeta Enterprise|ACUSDG0149</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Dinesh Sharma</t>
+          <t>Rajendra Singh</t>
         </is>
       </c>
       <c r="E95" t="n">
-        <v>7757</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="96">
@@ -2619,21 +2619,21 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>Rajasthan</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Suri Enterprises|ACUSD00062</t>
+          <t>Ravi Enterprises|ACUSDR0154</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Neeraj Kapoor</t>
+          <t>Yogesh Sharma</t>
         </is>
       </c>
       <c r="E96" t="n">
-        <v>2025</v>
+        <v>9843</v>
       </c>
     </row>
     <row r="97">
@@ -2642,17 +2642,17 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Rajasthan</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Swastik Enterprises|ACUSDS1206</t>
+          <t>Karni Traders|ACUSDK0094</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Jasbeer Verma</t>
+          <t>Ashish</t>
         </is>
       </c>
       <c r="E97" t="n">
@@ -2665,21 +2665,21 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Rajasthan</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Tirupati Agencies|ACUSDSS002</t>
+          <t>Rajlaxmi Enterprises|ACUSDJ0013</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Amit Patil</t>
+          <t>Subhash Yogi</t>
         </is>
       </c>
       <c r="E98" t="n">
-        <v>5082</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="99">
@@ -2688,21 +2688,21 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Uttarakhand</t>
+          <t>Rajasthan</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>V.S Enterprises|ACUSDV4827</t>
+          <t>Vinod Agency|ACUSDV0142</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Avneesh</t>
+          <t>Satish Singh</t>
         </is>
       </c>
       <c r="E99" t="n">
-        <v>2025</v>
+        <v>6530</v>
       </c>
     </row>
     <row r="100">
@@ -2711,17 +2711,17 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Rajasthan</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Varun Enterprises|ACUSDV0208</t>
+          <t>Rajeev Traders|ACUSDR0179</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Vinay Pandey</t>
+          <t>Rajendra Singh</t>
         </is>
       </c>
       <c r="E100" t="n">
@@ -2734,17 +2734,17 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Rajasthan</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Vinay Traders|ACUSDV0207</t>
+          <t>Baba Ramdev Distributors|ACUSDB0027</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Vinay Pandey</t>
+          <t>Atul</t>
         </is>
       </c>
       <c r="E101" t="n">
@@ -2757,17 +2757,17 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Rajasthan</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Vishal Traders|ACUSDV0085</t>
+          <t>Dv Trading Company|ACUSDD0103</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Jasbeer Verma</t>
+          <t>Lavish Sethi</t>
         </is>
       </c>
       <c r="E102" t="n">
@@ -2780,17 +2780,17 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Rajasthan</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Vishal Trading Co.|ACUSDV0079</t>
+          <t>I.G.Foods &amp; Snacks Ltd. (Conf)|ACUSDI0135</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Jasbeer Verma</t>
+          <t>Mahendra Pal Singh</t>
         </is>
       </c>
       <c r="E103" t="n">
@@ -2808,12 +2808,12 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Agrawal Traders|ACUSDA0168</t>
+          <t>Nls Brothers Private Limited|ACUSDNOO55</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Puneet Kansara</t>
+          <t>Mahendra Pal Singh</t>
         </is>
       </c>
       <c r="E104" t="n">
@@ -2831,12 +2831,12 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Arvind Agency|ACUSDA0106</t>
+          <t>Jyoti Enterprises|ACUSDJ1006</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Ajay Sachdeva / Ashu Tosh</t>
+          <t>Sarwan Sharma</t>
         </is>
       </c>
       <c r="E105" t="n">
@@ -2854,12 +2854,12 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Baba Ramdev Distributors|ACUSDB0027</t>
+          <t>Shri Shyam Trading Company|ACUSDS0441</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Lavish Sethi</t>
+          <t>Subhash Yogi</t>
         </is>
       </c>
       <c r="E106" t="n">
@@ -2877,12 +2877,12 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Baba Ramdev Distributors|ACUSDB0027</t>
+          <t>Agrawal Traders|ACUSDA0168</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Atul</t>
+          <t>Puneet Kansara</t>
         </is>
       </c>
       <c r="E107" t="n">
@@ -2900,12 +2900,12 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Dv Trading Company|ACUSDD0103</t>
+          <t>Arvind Agency|ACUSDA0106</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Atul</t>
+          <t>Ajay Sachdeva / Ashu Tosh</t>
         </is>
       </c>
       <c r="E108" t="n">
@@ -2923,12 +2923,12 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Dv Trading Company|ACUSDD0103</t>
+          <t>Satnam Traders|ACUSDS0269</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Lavish Sethi</t>
+          <t>Subhash Yogi</t>
         </is>
       </c>
       <c r="E109" t="n">
@@ -2946,16 +2946,16 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Geeta Enterprise|ACUSDG0149</t>
+          <t>Dv Trading Company|ACUSDD0103</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Rajendra Singh</t>
+          <t>Cp Gaur</t>
         </is>
       </c>
       <c r="E110" t="n">
-        <v>2025</v>
+        <v>7301</v>
       </c>
     </row>
     <row r="111">
@@ -2969,12 +2969,12 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>I.G.Foods &amp; Snacks Ltd. (Conf)|ACUSDI0135</t>
+          <t>Baba Ramdev Distributors|ACUSDB0027</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Mahendra Pal Singh</t>
+          <t>Lavish Sethi</t>
         </is>
       </c>
       <c r="E111" t="n">
@@ -2987,17 +2987,17 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Uttarakhand</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Jai Shankar Agency|ACUSDJ0595</t>
+          <t>Ravi Sons Enterprises|ACUSDR0205</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Dilip Rinuwa</t>
+          <t>Prakash Lohani</t>
         </is>
       </c>
       <c r="E112" t="n">
@@ -3010,17 +3010,17 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Uttarakhand</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Jyoti Enterprises|ACUSDJ1006</t>
+          <t>Durga Enterprises (Rishikesh)|ACUSDS0457</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Dilip Rinuwa</t>
+          <t>Avneesh</t>
         </is>
       </c>
       <c r="E113" t="n">
@@ -3033,17 +3033,17 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Uttarakhand</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Karni Traders|ACUSDK0094</t>
+          <t>Mishra Traders- Chamoli(Dewal)|ACUSDM0228</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Atul</t>
+          <t>Premdeep Deshwal</t>
         </is>
       </c>
       <c r="E114" t="n">
@@ -3056,17 +3056,17 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Uttarakhand</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Manoj Trading Company|ACUSDM0073</t>
+          <t>Deepak Agency|ACUSDD0543</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Subhash Yogi</t>
+          <t>Prakash Lohani</t>
         </is>
       </c>
       <c r="E115" t="n">
@@ -3079,17 +3079,17 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Uttarakhand</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>New Sunrise Agency|ACUSDN0605</t>
+          <t>Shree Ganesh Agency|ACUSDS1001</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Puneet Kansara</t>
+          <t>Salabh Partap</t>
         </is>
       </c>
       <c r="E116" t="n">
@@ -3102,21 +3102,21 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Uttarakhand</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Palak Agency|ACUSDP0178</t>
+          <t>Naman Agency|ACUSDN0028</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Satish Singh</t>
+          <t>Avneesh</t>
         </is>
       </c>
       <c r="E117" t="n">
-        <v>6530</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="118">
@@ -3125,17 +3125,17 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Uttarakhand</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Rajeev Traders|ACUSDR0179</t>
+          <t>V.S Enterprises|ACUSDV4827</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Rajendra Singh</t>
+          <t>Avneesh</t>
         </is>
       </c>
       <c r="E118" t="n">
@@ -3148,17 +3148,17 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Uttarakhand</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Rajlaxmi Enterprises|ACUSDJ0013</t>
+          <t>Pradeep Agency|ACUSDP4808</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Subhash Yogi</t>
+          <t>Prakash Lohani</t>
         </is>
       </c>
       <c r="E119" t="n">
@@ -3171,17 +3171,17 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Uttarakhand</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Rasik Remedies Pvt. Ltd.|ACUSDR0074</t>
+          <t>Hari Enterprises|ACUSDH0073</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Vacant Yogesh</t>
+          <t>Salabh Partap</t>
         </is>
       </c>
       <c r="E120" t="n">
@@ -3194,17 +3194,17 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Uttarakhand</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Ravi Enterprises|ACUSDR0154</t>
+          <t>Ankit Kumar &amp; Brothers|ACUSDA0797</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Vacant Yogesh</t>
+          <t>Avneesh</t>
         </is>
       </c>
       <c r="E121" t="n">
@@ -3217,21 +3217,21 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Uttarakhand</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Satnam Traders|ACUSDS0269</t>
+          <t>Shyam Sunder Enterprises- Pithoragarh|ACUSDS0462</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Subhash Yogi</t>
+          <t>Vacant</t>
         </is>
       </c>
       <c r="E122" t="n">
-        <v>2025</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="123">
@@ -3240,17 +3240,17 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Uttarakhand</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Shri Shyam Agency|ACUSDS4818</t>
+          <t>Shyam Sunder Enterprises- Pithoragarh|ACUSDS0462</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Mahendra Pal Singh</t>
+          <t>Prakash Lohani</t>
         </is>
       </c>
       <c r="E123" t="n">
@@ -3263,17 +3263,17 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>Uttarakhand</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Shri Vidhan Agency|ACUSDS0364</t>
+          <t>Shree Balaji Sales|ACUSDS0202</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Ajay Sachdeva / Ashu Tosh</t>
+          <t>Salabh Partap</t>
         </is>
       </c>
       <c r="E124" t="n">
@@ -3284,46 +3284,11 @@
       <c r="A125" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>Rajasthan</t>
-        </is>
-      </c>
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>Siddhi Vinayak Sales|ACUSDS4597</t>
-        </is>
-      </c>
-      <c r="D125" t="inlineStr">
-        <is>
-          <t>Mahendra Pal Singh</t>
-        </is>
-      </c>
+      <c r="B125" t="inlineStr"/>
+      <c r="C125" t="inlineStr"/>
+      <c r="D125" t="inlineStr"/>
       <c r="E125" t="n">
         <v>2025</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" s="1" t="n">
-        <v>124</v>
-      </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>Rajasthan</t>
-        </is>
-      </c>
-      <c r="C126" t="inlineStr">
-        <is>
-          <t>Vinod Agency|ACUSDV0142</t>
-        </is>
-      </c>
-      <c r="D126" t="inlineStr">
-        <is>
-          <t>Satish Singh</t>
-        </is>
-      </c>
-      <c r="E126" t="n">
-        <v>6530</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
asm Review file done week 1
</commit_message>
<xml_diff>
--- a/password.xlsx
+++ b/password.xlsx
@@ -852,17 +852,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Vishal Traders|ACUSDV0085</t>
+          <t>Anand Sales|ACUSDA0820</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Jasbeer Verma</t>
+          <t>Neeraj Kapoor</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -880,12 +880,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Ashish &amp; Co.|ACUSDA1159</t>
+          <t>Vishal Traders|ACUSDV0085</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Badal Srivastava</t>
+          <t>Jasbeer Verma</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -903,12 +903,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>P.R.Sales Agency|ACUSDP0142</t>
+          <t>Ashish &amp; Co.|ACUSDA1159</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Rakesh Kumar</t>
+          <t>Badal Srivastava</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -926,12 +926,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Swastik Enterprises|ACUSDS1206</t>
+          <t>P.R.Sales Agency|ACUSDP0142</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Jasbeer Verma</t>
+          <t>Rakesh Kumar</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -949,12 +949,12 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Dalal Trading Co.|ACUSDD1126</t>
+          <t>Swastik Enterprises|ACUSDS1206</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Yogesh</t>
+          <t>Jasbeer Verma</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -972,12 +972,12 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Shri Radhey Krishna Trading Co.|ACUSDS1204</t>
+          <t>Dalal Trading Co.|ACUSDD1126</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Jasbeer Verma</t>
+          <t>Yogesh</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -995,12 +995,12 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Vishal Trading Co.|ACUSDV0079</t>
+          <t>Shri Radhey Krishna Trading Co.|ACUSDS1204</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Pradeep Kumar</t>
+          <t>Jasbeer Verma</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -1018,12 +1018,12 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Shubham Overseas|ACUSDS1407</t>
+          <t>Vishal Trading Co.|ACUSDV0079</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Yogesh</t>
+          <t>Pradeep Kumar</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -1041,12 +1041,12 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Rameshwarm Enterprises|ACUSDR4921</t>
+          <t>Shubham Overseas|ACUSDS1407</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Ajit Pal</t>
+          <t>Yogesh</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -1064,12 +1064,12 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Pulkit Trading Co.|ACUSDP0132</t>
+          <t>Rameshwarm Enterprises|ACUSDR4921</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Badal Srivastava</t>
+          <t>Ajit Pal</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -1087,12 +1087,12 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Paras Kumar Satish Kr|ACUSDP0929</t>
+          <t>Pulkit Trading Co.|ACUSDP0132</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Rakesh Kumar</t>
+          <t>Badal Srivastava</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1110,12 +1110,12 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Murli Wala Sales|ACUSDM0200</t>
+          <t>Paras Kumar Satish Kr|ACUSDP0929</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Mahesh</t>
+          <t>Rakesh Kumar</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -1133,12 +1133,12 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Kalyani Trading Co.|ACUSDK0087</t>
+          <t>Murli Wala Sales|ACUSDM0200</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Ajit Pal</t>
+          <t>Mahesh</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -1156,12 +1156,12 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Harshit Trading Com|ACUSDY0005</t>
+          <t>Kalyani Trading Co.|ACUSDK0087</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Badal Srivastava</t>
+          <t>Ajit Pal</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -1179,12 +1179,12 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Ravindra Associates|ACUSDR0520</t>
+          <t>Harshit Trading Com|ACUSDY0005</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Yogesh</t>
+          <t>Badal Srivastava</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1202,12 +1202,12 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Shakshi Enterprises|ACUSDS0338</t>
+          <t>Ravindra Associates|ACUSDR0520</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Jasbeer Verma</t>
+          <t>Yogesh</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -1225,12 +1225,12 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Jai Shri Shyam Traders|LCLSOJ0054</t>
+          <t>Shakshi Enterprises|ACUSDS0338</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Yogesh</t>
+          <t>Jasbeer Verma</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1248,7 +1248,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Maruti Enterprises|ACUSDM0088</t>
+          <t>Jai Shri Shyam Traders|LCLSOJ0054</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1266,17 +1266,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Deepak Enterprises|ACUSDD0616</t>
+          <t>Maruti Enterprises|ACUSDM0088</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Parmod Kumar</t>
+          <t>Yogesh</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -1294,7 +1294,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Katna Sales|ACUSDK0086</t>
+          <t>Deepak Enterprises|ACUSDD0616</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1317,7 +1317,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Rattanchand And Sons|ACUSDR0130</t>
+          <t>Katna Sales|ACUSDK0086</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1340,7 +1340,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Amar Nath Harishchand|ACUSDA0133</t>
+          <t>Rattanchand And Sons|ACUSDR0130</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1363,7 +1363,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Shashank Enteprises|ACUSDS4809</t>
+          <t>Amar Nath Harishchand|ACUSDA0133</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1381,17 +1381,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Vinay Traders|ACUSDV0207</t>
+          <t>Shashank Enteprises|ACUSDS4809</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Vinay Pandey</t>
+          <t>Parmod Kumar</t>
         </is>
       </c>
       <c r="E42" t="n">
@@ -1409,12 +1409,12 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Anant Wardrobe|ACUSD00073</t>
+          <t>Vinay Traders|ACUSDV0207</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Brajesh Sharma</t>
+          <t>Vinay Pandey</t>
         </is>
       </c>
       <c r="E43" t="n">
@@ -1547,12 +1547,12 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Aakash Trading Co|ACUSDA0830</t>
+          <t>Anant Wardrobe|ACUSD00073</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Ankit Bhardwaj</t>
+          <t>Brajesh Sharma</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -1570,12 +1570,12 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Churaman Biharilal Asati|ACUSDC0531</t>
+          <t>Aakash Trading Co|ACUSDA0830</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Anand Gupta</t>
+          <t>Ankit Bhardwaj</t>
         </is>
       </c>
       <c r="E50" t="n">
@@ -1593,12 +1593,12 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Varun Enterprises|ACUSDV0208</t>
+          <t>Churaman Biharilal Asati|ACUSDC0531</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Vinay Pandey</t>
+          <t>Anand Gupta</t>
         </is>
       </c>
       <c r="E51" t="n">
@@ -1616,12 +1616,12 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Amit Sales|ACUSDA0137</t>
+          <t>Varun Enterprises|ACUSDV0208</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Anand Gupta</t>
+          <t>Vinay Pandey</t>
         </is>
       </c>
       <c r="E52" t="n">
@@ -1639,12 +1639,12 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Shanti Marketing|ACUSDS4808</t>
+          <t>Amit Sales|ACUSDA0137</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Vinay Pandey</t>
+          <t>Anand Gupta</t>
         </is>
       </c>
       <c r="E53" t="n">
@@ -1662,12 +1662,12 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Abhinandan Enterprises|ACUSDA0088</t>
+          <t>Shanti Marketing|ACUSDS4808</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Brajesh Sharma</t>
+          <t>Vinay Pandey</t>
         </is>
       </c>
       <c r="E54" t="n">
@@ -1685,12 +1685,12 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>O.S. Agency|ACUSDO0028</t>
+          <t>Abhinandan Enterprises|ACUSDA0088</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Vinay Pandey</t>
+          <t>Brajesh Sharma</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>R.D. Plastic|ACUSDR0127</t>
+          <t>O.S. Agency|ACUSDO0028</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1731,12 +1731,12 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Krishna Enterprises|</t>
+          <t>R.D. Plastic|ACUSDR0127</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Ankit Bhardwaj</t>
+          <t>Vinay Pandey</t>
         </is>
       </c>
       <c r="E57" t="n">
@@ -1754,7 +1754,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Aggarwal Agency|ACUSDA0410</t>
+          <t>Krishna Enterprises|</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1777,12 +1777,12 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Bhagwan Das Kirana And General Store|</t>
+          <t>Aggarwal Agency|ACUSDA0410</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Vinay Pandey</t>
+          <t>Ankit Bhardwaj</t>
         </is>
       </c>
       <c r="E59" t="n">
@@ -1803,7 +1803,11 @@
           <t>Bhagwan Das Kirana And General Store|</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr"/>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Vinay Pandey</t>
+        </is>
+      </c>
       <c r="E60" t="n">
         <v>2025</v>
       </c>
@@ -1819,14 +1823,10 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Reliable Industry|ACUSDR0204</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>Vinay Pandey</t>
-        </is>
-      </c>
+          <t>Bhagwan Das Kirana And General Store|</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr"/>
       <c r="E61" t="n">
         <v>2025</v>
       </c>
@@ -1837,17 +1837,17 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Prabhat Agency|ACUSDP2385</t>
+          <t>Reliable Industry|ACUSDR0204</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Rakesh Tripathi</t>
+          <t>Vinay Pandey</t>
         </is>
       </c>
       <c r="E62" t="n">
@@ -1865,16 +1865,16 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Prabhat Trading Com.|ACUSDP0183</t>
+          <t>Prabhat Agency|ACUSDP2385</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Anil Jamadar Singh</t>
+          <t>Rakesh Tripathi</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>5808</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="64">
@@ -1888,16 +1888,16 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Adhira Agency|ACUSDSS005</t>
+          <t>Prabhat Trading Com.|ACUSDP0183</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Anil Jamadar Singh</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>1164</v>
+        <v>5808</v>
       </c>
     </row>
     <row r="65">
@@ -1911,16 +1911,16 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Optimize Crusder|ACUSDO0026</t>
+          <t>Adhira Agency|ACUSDSS005</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Kapil Sharma</t>
+          <t>Vacant</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>4920</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="66">
@@ -1934,16 +1934,16 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Jainil Traders|ACUSDJ0023</t>
+          <t>Optimize Crusder|ACUSDO0026</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Kapil Sharma</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>1164</v>
+        <v>4920</v>
       </c>
     </row>
     <row r="67">
@@ -1957,7 +1957,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Krishna Agencies|ACUSDSS003</t>
+          <t>Jainil Traders|ACUSDJ0023</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -1980,16 +1980,16 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Bharat Traders|ACUSDB0039</t>
+          <t>Krishna Agencies|ACUSDSS003</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Kapil Sharma</t>
+          <t>Vacant</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>4920</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="69">
@@ -2003,16 +2003,16 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>J.K. Brothers|ACUSDJ4838</t>
+          <t>Bharat Traders|ACUSDB0039</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Kapil Sharma</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>1164</v>
+        <v>4920</v>
       </c>
     </row>
     <row r="70">
@@ -2026,7 +2026,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Jai Mata Di Agency|ACUSDSS001</t>
+          <t>J.K. Brothers|ACUSDJ4838</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2049,16 +2049,16 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Sunrise Enterprises|ACUSDS0771</t>
+          <t>Jai Mata Di Agency|ACUSDSS001</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Dinesh Sharma</t>
+          <t>Vacant</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>7757</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="72">
@@ -2072,16 +2072,16 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Nidhi Sales|ACUSDN4807</t>
+          <t>Sunrise Enterprises|ACUSDS0771</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Anil Jamadar Singh</t>
+          <t>Dinesh Sharma</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>5808</v>
+        <v>7757</v>
       </c>
     </row>
     <row r="73">
@@ -2095,16 +2095,16 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Krishna Marketing|ACUSDSS006</t>
+          <t>Nidhi Sales|ACUSDN4807</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Anil Jamadar Singh</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>1164</v>
+        <v>5808</v>
       </c>
     </row>
     <row r="74">
@@ -2118,16 +2118,16 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Ajinkya Traders|ACUSDA0146</t>
+          <t>Krishna Marketing|ACUSDSS006</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Shailesh Surve</t>
+          <t>Vacant</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>7136</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="75">
@@ -2141,16 +2141,16 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Tirupati Agencies|ACUSDSS002</t>
+          <t>Ajinkya Traders|ACUSDA0146</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Rakesh Tripathi</t>
+          <t>Shailesh Surve</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>2025</v>
+        <v>7136</v>
       </c>
     </row>
     <row r="76">
@@ -2164,7 +2164,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Shree Datta Agency|ACUSDSS004</t>
+          <t>Tirupati Agencies|ACUSDSS002</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2187,16 +2187,16 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Navinya Enterprises|ACUSDN0052</t>
+          <t>Shree Datta Agency|ACUSDSS004</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Shailesh Surve</t>
+          <t>Rakesh Tripathi</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>7136</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="78">
@@ -2205,21 +2205,21 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Garg Sales Corporation|ACUSDG1091</t>
+          <t>Navinya Enterprises|ACUSDN0052</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Neeraj Kapoor</t>
+          <t>Shailesh Surve</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>2025</v>
+        <v>7136</v>
       </c>
     </row>
     <row r="79">
@@ -2233,12 +2233,12 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Bajarang Sweet House (Conf)|ACUSDB0963</t>
+          <t>Garg Sales Corporation|ACUSDG1091</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Jasbir Verma</t>
+          <t>Neeraj Kapoor</t>
         </is>
       </c>
       <c r="E79" t="n">
@@ -2256,7 +2256,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Sant Enterprises|ACUSDS1100</t>
+          <t>Bajarang Sweet House (Conf)|ACUSDB0963</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2279,12 +2279,12 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Shivam Agency|ACUSDSS896</t>
+          <t>Sant Enterprises|ACUSDS1100</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Rajinder Singh</t>
+          <t>Jasbir Verma</t>
         </is>
       </c>
       <c r="E81" t="n">
@@ -2302,12 +2302,12 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Jeet Ram And Sons|ACUSD00063</t>
+          <t>Shivam Agency|ACUSDSS896</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Neeraj Kapoor</t>
+          <t>Pradeep</t>
         </is>
       </c>
       <c r="E82" t="n">
@@ -2325,12 +2325,12 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Commander Trade Link|ACUSDC1514</t>
+          <t>Jeet Ram And Sons|ACUSD00063</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Jasbir Verma</t>
+          <t>Neeraj Kapoor</t>
         </is>
       </c>
       <c r="E83" t="n">
@@ -2348,12 +2348,12 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Saurabh Traders|ACUSDSS106</t>
+          <t>Commander Trade Link|ACUSDC1514</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Rajinder Singh</t>
+          <t>Jasbir Verma</t>
         </is>
       </c>
       <c r="E84" t="n">
@@ -2371,12 +2371,12 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Suri Enterprises|ACUSD00062</t>
+          <t>Saurabh Traders|ACUSDSS106</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Neeraj Kapoor</t>
+          <t>Pradeep</t>
         </is>
       </c>
       <c r="E85" t="n">
@@ -2394,12 +2394,12 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Grace Drinks Pvt Ltd|ACUSDG0174</t>
+          <t>Suri Enterprises|ACUSD00062</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Shymu Verma</t>
+          <t>Pradeep</t>
         </is>
       </c>
       <c r="E86" t="n">
@@ -2417,12 +2417,12 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Suri Enterprises|ACUSD00062</t>
+          <t>Grace Drinks Pvt Ltd|ACUSDG0174</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Shymu Verma</t>
+          <t>Rohit Medirata</t>
         </is>
       </c>
       <c r="E87" t="n">
@@ -2440,7 +2440,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Anand Sales|ACUSDA0820</t>
+          <t>Bhana Ram &amp; Sons|ACUSDB0473</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2463,7 +2463,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Bhana Ram &amp; Sons|ACUSDB0473</t>
+          <t>Grace Drinks Pvt Ltd|ACUSDG0174</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">

</xml_diff>

<commit_message>
4th week update done
</commit_message>
<xml_diff>
--- a/password.xlsx
+++ b/password.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E123"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,7 +489,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Shree Ji Enterprises|ACUSDS0174</t>
+          <t>Parshvanath Sales Agency|ACUSDP0211</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -512,16 +512,16 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Ishan Marketing|ACUSDI9604</t>
+          <t>Raj Sales|ACUSDR4923</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Toshif Mansuri</t>
+          <t>Hitesh Thakker</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>9989</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="5">
@@ -535,16 +535,16 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ashok Traders|ACUSDA0117</t>
+          <t>C.J.Malaviya &amp; Co.|ACUSDC0049</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Toshif Mansuri</t>
+          <t>Hitesh Thakker</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>9989</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="6">
@@ -553,21 +553,21 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Khemani Enetrprises (Conf)|ACUSDK2024</t>
+          <t>Satnam Sales|AQUSDK2024</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Yogesh</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>1164</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="7">
@@ -576,21 +576,21 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Proline Sales Agency|ACUSDP5556</t>
+          <t>Shakshi Enterprises|ACUSDS0338</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Jasbeer Verma</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>1164</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="8">
@@ -599,21 +599,21 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Farr Ayo Distribution|ACUSDF0061</t>
+          <t>Jai Shri Shyam Traders|LCLSOJ0054</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Girvat Raj</t>
+          <t>Yogesh</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>4370</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="9">
@@ -622,21 +622,21 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Parshvanath Sales Agency|ACUSDP0211</t>
+          <t>Maruti Enterprises|ACUSDM0088</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Hitesh Thakker</t>
+          <t>Yogesh</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>1827</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="10">
@@ -645,21 +645,21 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Joshi Enterprises|ACUSDJ0572</t>
+          <t>Vinay Traders|ACUSDV0207</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Vinay Pandey</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>1164</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="11">
@@ -668,21 +668,21 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Raj Sales|ACUSDR4923</t>
+          <t>Naman Enterprises|ACUSDN1114</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Hitesh Thakker</t>
+          <t>Anand Gupta</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1827</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="12">
@@ -691,21 +691,21 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>C.J.Malaviya &amp; Co.|ACUSDC0049</t>
+          <t>Anant Wardrobe|ACUSD00073</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Hitesh Thakker</t>
+          <t>Brajesh Sharma</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1827</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="13">
@@ -714,21 +714,21 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Somnath Ji Traders|ACUSDS4925</t>
+          <t>O.S. Agency|ACUSDO0028</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Sahil Mansuri</t>
+          <t>Vinay Pandey</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>4760</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="14">
@@ -737,21 +737,21 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Satnam Sales|AQUSDK2024</t>
+          <t>Jainil Traders|ACUSDJ0023</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Yogesh</t>
+          <t>Vacant</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>2025</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="15">
@@ -760,17 +760,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Madhu Enterprises|ACUSDM0117</t>
+          <t>Prabhat Agency|ACUSDP2385</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Ajit Pal</t>
+          <t>Rakesh Tripathi</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -783,21 +783,21 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Hoseiry House|ACUSDH4804</t>
+          <t>Krishna Marketing|ACUSDSS006</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Ajit Pal</t>
+          <t>Vacant</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>2025</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="17">
@@ -806,17 +806,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Shree Kanha Ji Marketing|ACUSDS0438</t>
+          <t>Tirupati Agencies|ACUSDSS002</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Rajiv Kumar</t>
+          <t>Rakesh Tripathi</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -829,17 +829,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Shreyansh Marketing|ACUSDS0070</t>
+          <t>Shree Datta Agency|ACUSDSS004</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Mahesh</t>
+          <t>Rakesh Tripathi</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -857,7 +857,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Anand Sales|ACUSDA0820</t>
+          <t>Garg Sales Corporation|ACUSDG1091</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -875,17 +875,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Uttarakhand</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Vishal Traders|ACUSDV0085</t>
+          <t>Ankit Kumar &amp; Brothers|ACUSDA0797</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Jasbeer Verma</t>
+          <t>Avneesh</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -898,21 +898,21 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Ashish &amp; Co.|ACUSDA1159</t>
+          <t>Shree Ji Enterprises|ACUSDS0174</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Badal Srivastava</t>
+          <t>Hitesh Thakker</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>2025</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="22">
@@ -921,21 +921,21 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>P.R.Sales Agency|ACUSDP0142</t>
+          <t>Ishan Marketing|ACUSDI9604</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Rakesh Kumar</t>
+          <t>Toshif Mansuri</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>2025</v>
+        <v>9989</v>
       </c>
     </row>
     <row r="23">
@@ -944,21 +944,21 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Swastik Enterprises|ACUSDS1206</t>
+          <t>Ashok Traders|ACUSDA0117</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Jasbeer Verma</t>
+          <t>Toshif Mansuri</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>2025</v>
+        <v>9989</v>
       </c>
     </row>
     <row r="24">
@@ -967,17 +967,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Dalal Trading Co.|ACUSDD1126</t>
+          <t>Khemani Enetrprises (Conf)|ACUSDK2024</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Yogesh</t>
+          <t>Jatin Jain</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -990,17 +990,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Shri Radhey Krishna Trading Co.|ACUSDS1204</t>
+          <t>Proline Sales Agency|ACUSDP5556</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Jasbeer Verma</t>
+          <t>Jatin Jain</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -1013,21 +1013,21 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Vishal Trading Co.|ACUSDV0079</t>
+          <t>Farr Ayo Distribution|ACUSDF0061</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Pradeep Kumar</t>
+          <t>Girvat Raj</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>2025</v>
+        <v>4370</v>
       </c>
     </row>
     <row r="27">
@@ -1036,21 +1036,21 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Shubham Overseas|ACUSDS1407</t>
+          <t>Joshi Enterprises|ACUSDJ0572</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Yogesh</t>
+          <t>Vacant</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>2025</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="28">
@@ -1059,21 +1059,21 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Rameshwarm Enterprises|ACUSDR4921</t>
+          <t>Somnath Ji Traders|ACUSDS4925</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Ajit Pal</t>
+          <t>Sahil Mansuri</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>2025</v>
+        <v>4760</v>
       </c>
     </row>
     <row r="29">
@@ -1087,12 +1087,12 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Pulkit Trading Co.|ACUSDP0132</t>
+          <t>Madhu Enterprises|ACUSDM0117</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Badal Srivastava</t>
+          <t>Ajit Pal</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1110,12 +1110,12 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Paras Kumar Satish Kr|ACUSDP0929</t>
+          <t>Hoseiry House|ACUSDH4804</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Rakesh Kumar</t>
+          <t>Ajit Pal</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -1133,12 +1133,12 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Murli Wala Sales|ACUSDM0200</t>
+          <t>Shree Kanha Ji Marketing|ACUSDS0438</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Mahesh</t>
+          <t>Rajiv Kumar</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -1156,12 +1156,12 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Kalyani Trading Co.|ACUSDK0087</t>
+          <t>Shreyansh Marketing|ACUSDS0070</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Ajit Pal</t>
+          <t>Mahesh</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -1174,17 +1174,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Harshit Trading Com|ACUSDY0005</t>
+          <t>Anand Sales|ACUSDA0820</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Badal Srivastava</t>
+          <t>Neeraj Kapoor</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1202,12 +1202,12 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Ravindra Associates|ACUSDR0520</t>
+          <t>Vishal Traders|ACUSDV0085</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Yogesh</t>
+          <t>Jasbeer Verma</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -1225,12 +1225,12 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Shakshi Enterprises|ACUSDS0338</t>
+          <t>Ashish &amp; Co.|ACUSDA1159</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Jasbeer Verma</t>
+          <t>Badal Srivastava</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1248,12 +1248,12 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Jai Shri Shyam Traders|LCLSOJ0054</t>
+          <t>P.R.Sales Agency|ACUSDP0142</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Yogesh</t>
+          <t>Rakesh Kumar</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -1271,12 +1271,12 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Maruti Enterprises|ACUSDM0088</t>
+          <t>Swastik Enterprises|ACUSDS1206</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Yogesh</t>
+          <t>Jasbeer Verma</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -1289,17 +1289,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Deepak Enterprises|ACUSDD0616</t>
+          <t>Dalal Trading Co.|ACUSDD1126</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Parmod Kumar</t>
+          <t>Yogesh</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -1312,17 +1312,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Katna Sales|ACUSDK0086</t>
+          <t>Shri Radhey Krishna Trading Co.|ACUSDS1204</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Parmod Kumar</t>
+          <t>Jasbeer Verma</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -1335,17 +1335,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Rattanchand And Sons|ACUSDR0130</t>
+          <t>Vishal Trading Co.|ACUSDV0079</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Parmod Kumar</t>
+          <t>Pradeep Kumar</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1358,17 +1358,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Amar Nath Harishchand|ACUSDA0133</t>
+          <t>Shubham Overseas|ACUSDS1407</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Parmod Kumar</t>
+          <t>Yogesh</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1381,17 +1381,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Shashank Enteprises|ACUSDS4809</t>
+          <t>Rameshwarm Enterprises|ACUSDR4921</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Parmod Kumar</t>
+          <t>Ajit Pal</t>
         </is>
       </c>
       <c r="E42" t="n">
@@ -1404,17 +1404,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Vinay Traders|ACUSDV0207</t>
+          <t>Pulkit Trading Co.|ACUSDP0132</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Vinay Pandey</t>
+          <t>Badal Srivastava</t>
         </is>
       </c>
       <c r="E43" t="n">
@@ -1427,17 +1427,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Shree Gopalji Enterprises|ACUSDS2806</t>
+          <t>Paras Kumar Satish Kr|ACUSDP0929</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Ankit Bhardwaj</t>
+          <t>Rakesh Kumar</t>
         </is>
       </c>
       <c r="E44" t="n">
@@ -1450,17 +1450,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Barsaiya Traders|ACUSDB0005</t>
+          <t>Murli Wala Sales|ACUSDM0200</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Vinay Pandey</t>
+          <t>Mahesh</t>
         </is>
       </c>
       <c r="E45" t="n">
@@ -1473,17 +1473,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Goyal Marketing|ACUSDG0603</t>
+          <t>Kalyani Trading Co.|ACUSDK0087</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Ankit Bhardwaj</t>
+          <t>Ajit Pal</t>
         </is>
       </c>
       <c r="E46" t="n">
@@ -1496,17 +1496,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Parvati Agency|ACUSDP4826</t>
+          <t>Harshit Trading Com|ACUSDY0005</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Ankit Bhardwaj</t>
+          <t>Badal Srivastava</t>
         </is>
       </c>
       <c r="E47" t="n">
@@ -1519,17 +1519,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Naman Enterprises|ACUSDN1114</t>
+          <t>Ravindra Associates|ACUSDR0520</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Anand Gupta</t>
+          <t>Rakesh Kumar</t>
         </is>
       </c>
       <c r="E48" t="n">
@@ -1542,17 +1542,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Anant Wardrobe|ACUSD00073</t>
+          <t>Deepak Enterprises|ACUSDD0616</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Brajesh Sharma</t>
+          <t>Parmod Kumar</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -1565,17 +1565,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Aakash Trading Co|ACUSDA0830</t>
+          <t>Katna Sales|ACUSDK0086</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Ankit Bhardwaj</t>
+          <t>Parmod Kumar</t>
         </is>
       </c>
       <c r="E50" t="n">
@@ -1588,17 +1588,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Churaman Biharilal Asati|ACUSDC0531</t>
+          <t>Rattanchand And Sons|ACUSDR0130</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Anand Gupta</t>
+          <t>Parmod Kumar</t>
         </is>
       </c>
       <c r="E51" t="n">
@@ -1611,17 +1611,17 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Varun Enterprises|ACUSDV0208</t>
+          <t>Amar Nath Harishchand|ACUSDA0133</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Vinay Pandey</t>
+          <t>Parmod Kumar</t>
         </is>
       </c>
       <c r="E52" t="n">
@@ -1634,17 +1634,17 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Amit Sales|ACUSDA0137</t>
+          <t>Shashank Enteprises|ACUSDS4809</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Anand Gupta</t>
+          <t>Parmod Kumar</t>
         </is>
       </c>
       <c r="E53" t="n">
@@ -1662,12 +1662,12 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Shanti Marketing|ACUSDS4808</t>
+          <t>Shree Gopalji Enterprises|ACUSDS2806</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Vinay Pandey</t>
+          <t>Ankit Bhardwaj</t>
         </is>
       </c>
       <c r="E54" t="n">
@@ -1685,12 +1685,12 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Abhinandan Enterprises|ACUSDA0088</t>
+          <t>Barsaiya Traders|ACUSDB0005</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Brajesh Sharma</t>
+          <t>Vinay Pandey</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -1708,12 +1708,12 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>O.S. Agency|ACUSDO0028</t>
+          <t>Goyal Marketing|ACUSDG0603</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Vinay Pandey</t>
+          <t>Ankit Bhardwaj</t>
         </is>
       </c>
       <c r="E56" t="n">
@@ -1731,12 +1731,12 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>R.D. Plastic|ACUSDR0127</t>
+          <t>Parvati Agency|ACUSDP4826</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Vinay Pandey</t>
+          <t>Ankit Bhardwaj</t>
         </is>
       </c>
       <c r="E57" t="n">
@@ -1754,7 +1754,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Krishna Enterprises|</t>
+          <t>Aakash Trading Co|ACUSDA0830</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1777,12 +1777,12 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Aggarwal Agency|ACUSDA0410</t>
+          <t>Churaman Biharilal Asati|ACUSDC0531</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Ankit Bhardwaj</t>
+          <t>Anand Gupta</t>
         </is>
       </c>
       <c r="E59" t="n">
@@ -1800,7 +1800,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Bhagwan Das Kirana And General Store|</t>
+          <t>Varun Enterprises|ACUSDV0208</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1823,10 +1823,14 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Bhagwan Das Kirana And General Store|</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr"/>
+          <t>Amit Sales|ACUSDA0137</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Anand Gupta</t>
+        </is>
+      </c>
       <c r="E61" t="n">
         <v>2025</v>
       </c>
@@ -1842,7 +1846,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Reliable Industry|ACUSDR0204</t>
+          <t>Shanti Marketing|ACUSDS4808</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1860,17 +1864,17 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Prabhat Agency|ACUSDP2385</t>
+          <t>Abhinandan Enterprises|ACUSDA0088</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Rakesh Tripathi</t>
+          <t>Brajesh Sharma</t>
         </is>
       </c>
       <c r="E63" t="n">
@@ -1883,21 +1887,21 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Prabhat Trading Com.|ACUSDP0183</t>
+          <t>R.D. Plastic|ACUSDR0127</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Anil Jamadar Singh</t>
+          <t>Vinay Pandey</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>5808</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="65">
@@ -1906,21 +1910,21 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Adhira Agency|ACUSDSS005</t>
+          <t>Krishna Enterprises|</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Ankit Bhardwaj</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>1164</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="66">
@@ -1929,21 +1933,21 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Optimize Crusder|ACUSDO0026</t>
+          <t>Aggarwal Agency|ACUSDA0410</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Kapil Sharma</t>
+          <t>Ankit Bhardwaj</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>4920</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="67">
@@ -1952,21 +1956,21 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Jainil Traders|ACUSDJ0023</t>
+          <t>Bhagwan Das Kirana And General Store|</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Vinay Pandey</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>1164</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="68">
@@ -1975,21 +1979,17 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Krishna Agencies|ACUSDSS003</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>Vacant</t>
-        </is>
-      </c>
+          <t>Bhagwan Das Kirana And General Store|</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr"/>
       <c r="E68" t="n">
-        <v>1164</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="69">
@@ -1998,21 +1998,21 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Bharat Traders|ACUSDB0039</t>
+          <t>Reliable Industry|ACUSDR0204</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Kapil Sharma</t>
+          <t>Vinay Pandey</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>4920</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="70">
@@ -2026,16 +2026,16 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>J.K. Brothers|ACUSDJ4838</t>
+          <t>Prabhat Trading Com.|ACUSDP0183</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Anil Jamadar Singh</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>1164</v>
+        <v>5808</v>
       </c>
     </row>
     <row r="71">
@@ -2049,7 +2049,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Jai Mata Di Agency|ACUSDSS001</t>
+          <t>Adhira Agency|ACUSDSS005</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2072,16 +2072,16 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Sunrise Enterprises|ACUSDS0771</t>
+          <t>Optimize Crusder|ACUSDO0026</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Dinesh Sharma</t>
+          <t>Kapil Sharma</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>7757</v>
+        <v>4920</v>
       </c>
     </row>
     <row r="73">
@@ -2095,16 +2095,16 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Nidhi Sales|ACUSDN4807</t>
+          <t>Krishna Agencies|ACUSDSS003</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Anil Jamadar Singh</t>
+          <t>Vacant</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>5808</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="74">
@@ -2118,16 +2118,16 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Krishna Marketing|ACUSDSS006</t>
+          <t>Bharat Traders|ACUSDB0039</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Vacant</t>
+          <t>Kapil Sharma</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>1164</v>
+        <v>4920</v>
       </c>
     </row>
     <row r="75">
@@ -2141,16 +2141,16 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Ajinkya Traders|ACUSDA0146</t>
+          <t>J.K. Brothers|ACUSDJ4838</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Shailesh Surve</t>
+          <t>Vacant</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>7136</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="76">
@@ -2164,16 +2164,16 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Tirupati Agencies|ACUSDSS002</t>
+          <t>Jai Mata Di Agency|ACUSDSS001</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Rakesh Tripathi</t>
+          <t>Vacant</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>2025</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="77">
@@ -2187,16 +2187,16 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Shree Datta Agency|ACUSDSS004</t>
+          <t>Sunrise Enterprises|ACUSDS0771</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Rakesh Tripathi</t>
+          <t>Dinesh Sharma</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>2025</v>
+        <v>7757</v>
       </c>
     </row>
     <row r="78">
@@ -2210,16 +2210,16 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Navinya Enterprises|ACUSDN0052</t>
+          <t>Nidhi Sales|ACUSDN4807</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Shailesh Surve</t>
+          <t>Anil Jamadar Singh</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>7136</v>
+        <v>5808</v>
       </c>
     </row>
     <row r="79">
@@ -2228,21 +2228,21 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Garg Sales Corporation|ACUSDG1091</t>
+          <t>Ajinkya Traders|ACUSDA0146</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Neeraj Kapoor</t>
+          <t>Shailesh Surve</t>
         </is>
       </c>
       <c r="E79" t="n">
-        <v>2025</v>
+        <v>7136</v>
       </c>
     </row>
     <row r="80">
@@ -2251,21 +2251,21 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>Maharashtra</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Bajarang Sweet House (Conf)|ACUSDB0963</t>
+          <t>Navinya Enterprises|ACUSDN0052</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Jasbir Verma</t>
+          <t>Shailesh Surve</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>2025</v>
+        <v>7136</v>
       </c>
     </row>
     <row r="81">
@@ -2279,7 +2279,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Sant Enterprises|ACUSDS1100</t>
+          <t>Bajarang Sweet House (Conf)|ACUSDB0963</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2302,12 +2302,12 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Shivam Agency|ACUSDSS896</t>
+          <t>Sant Enterprises|ACUSDS1100</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Pradeep</t>
+          <t>Jasbir Verma</t>
         </is>
       </c>
       <c r="E82" t="n">
@@ -2325,12 +2325,12 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Jeet Ram And Sons|ACUSD00063</t>
+          <t>Shivam Agency|ACUSDSS896</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Neeraj Kapoor</t>
+          <t>Pradeep</t>
         </is>
       </c>
       <c r="E83" t="n">
@@ -2348,12 +2348,12 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Commander Trade Link|ACUSDC1514</t>
+          <t>Jeet Ram And Sons|ACUSD00063</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Jasbir Verma</t>
+          <t>Neeraj Kapoor</t>
         </is>
       </c>
       <c r="E84" t="n">
@@ -2371,12 +2371,12 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Saurabh Traders|ACUSDSS106</t>
+          <t>Commander Trade Link|ACUSDC1514</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Pradeep</t>
+          <t>Jasbir Verma</t>
         </is>
       </c>
       <c r="E85" t="n">
@@ -2394,7 +2394,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Suri Enterprises|ACUSD00062</t>
+          <t>Saurabh Traders|ACUSDSS106</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2514,11 +2514,11 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Satish Singh</t>
+          <t>Rajendra Singh</t>
         </is>
       </c>
       <c r="E91" t="n">
-        <v>6530</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="92">
@@ -2560,7 +2560,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Sarwan Sharma</t>
+          <t>Dili Renua</t>
         </is>
       </c>
       <c r="E93" t="n">
@@ -2698,11 +2698,11 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Satish Singh</t>
+          <t>Rajendra Singh</t>
         </is>
       </c>
       <c r="E99" t="n">
-        <v>6530</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="100">
@@ -2859,7 +2859,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Sarwan Sharma</t>
+          <t>Dili Renua</t>
         </is>
       </c>
       <c r="E106" t="n">
@@ -3199,12 +3199,12 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Ankit Kumar &amp; Brothers|ACUSDA0797</t>
+          <t>Shyam Sunder Enterprises- Pithoragarh|ACUSDS0462</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Avneesh</t>
+          <t>Mahesh</t>
         </is>
       </c>
       <c r="E121" t="n">
@@ -3222,38 +3222,15 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Shyam Sunder Enterprises- Pithoragarh|ACUSDS0462</t>
+          <t>Shree Balaji Sales|ACUSDS0202</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Mahesh</t>
+          <t>Salabh Partap</t>
         </is>
       </c>
       <c r="E122" t="n">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" s="1" t="n">
-        <v>121</v>
-      </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>Uttarakhand</t>
-        </is>
-      </c>
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>Shree Balaji Sales|ACUSDS0202</t>
-        </is>
-      </c>
-      <c r="D123" t="inlineStr">
-        <is>
-          <t>Salabh Partap</t>
-        </is>
-      </c>
-      <c r="E123" t="n">
         <v>2025</v>
       </c>
     </row>

</xml_diff>